<commit_message>
update foto profil dan icon foto
</commit_message>
<xml_diff>
--- a/uploads/Laporan_kandidat.xlsx
+++ b/uploads/Laporan_kandidat.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Nama</t>
   </si>
@@ -53,10 +53,10 @@
     <t>nindy@gmail.com</t>
   </si>
   <si>
-    <t>wonosobo, 2000-02-18</t>
-  </si>
-  <si>
-    <t>RT04/RW04, KLEYANG GUNUNG, PUNGANGAN, IDANO GAWO, KABUPATEN NIAS, SUMATERA UTARA</t>
+    <t>Jakarta, 2025-10-29</t>
+  </si>
+  <si>
+    <t>RT04/RW04, KLEYANG GUNUNG, PUNGANGAN, BAWOLATO, KABUPATEN NIAS, SUMATERA UTARA</t>
   </si>
   <si>
     <t>098887990554</t>
@@ -65,22 +65,34 @@
     <t>AKTIF</t>
   </si>
   <si>
-    <t>IDA FANIA</t>
-  </si>
-  <si>
-    <t>Netral</t>
-  </si>
-  <si>
-    <t>idafania33@gmail.com</t>
-  </si>
-  <si>
-    <t>OFF</t>
-  </si>
-  <si>
     <t>LIA ETIKASARI</t>
   </si>
   <si>
     <t>liaetikasari0826@gmail.com</t>
+  </si>
+  <si>
+    <t>TEMANGGUNG, 2007-01-11</t>
+  </si>
+  <si>
+    <t>JL MELATI, BULU, KABUPATEN TEMANGGUNG, JAWA TENGAH</t>
+  </si>
+  <si>
+    <t>098776445667</t>
+  </si>
+  <si>
+    <t>KURNIA AINUN</t>
+  </si>
+  <si>
+    <t>kurnia@gmail.com</t>
+  </si>
+  <si>
+    <t>TEMANGGUNG, 2025-10-01</t>
+  </si>
+  <si>
+    <t>KRAJAN, KANDANGAN, KABUPATEN TEMANGGUNG, JAWA TENGAH</t>
+  </si>
+  <si>
+    <t>0998877765554</t>
   </si>
 </sst>
 </file>
@@ -428,9 +440,9 @@
     <col min="2" max="2" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="31" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="95" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="93" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -498,39 +510,55 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>6285158040206</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="D3">
-        <v>6289907711225</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>12345</v>
+      </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>6285158040206</v>
-      </c>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
+        <v>6256667889001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>90909</v>
+      </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
update footer dan maps
</commit_message>
<xml_diff>
--- a/uploads/Laporan_kandidat.xlsx
+++ b/uploads/Laporan_kandidat.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Nama</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>OFF</t>
+  </si>
+  <si>
+    <t>LIA ETIKASARI</t>
+  </si>
+  <si>
+    <t>liaetikasari0826@gmail.com</t>
+  </si>
+  <si>
+    <t>KURNIA AINUN</t>
+  </si>
+  <si>
+    <t>etikasarilia26@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -404,7 +416,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -412,9 +424,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="31" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="24" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="83" bestFit="true" customWidth="true" style="0"/>
@@ -493,6 +505,46 @@
       <c r="G3"/>
       <c r="I3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>85158040206</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>628885122711</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="I5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update lowongan kerja user
</commit_message>
<xml_diff>
--- a/uploads/Laporan_kandidat.xlsx
+++ b/uploads/Laporan_kandidat.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Nama</t>
   </si>
@@ -50,10 +50,10 @@
     <t>nindy@gmail.com</t>
   </si>
   <si>
-    <t>wonosobo, 2000-02-18</t>
-  </si>
-  <si>
-    <t>KENANGAN MANTAN, SINUNUKAN, KABUPATEN MANDAILING NATAL, SUMATERA UTARA</t>
+    <t>temanggung abc, 2000-02-18</t>
+  </si>
+  <si>
+    <t>KENANGAN MANTAN abcDE, SINUNUKAN, KABUPATEN MANDAILING NATAL, SUMATERA UTARA</t>
   </si>
   <si>
     <t>AKTIF</t>
@@ -62,25 +62,37 @@
     <t>IDA FANIA</t>
   </si>
   <si>
+    <t>idafania33@gmail.com</t>
+  </si>
+  <si>
+    <t>Jakarta, 2025-11-06</t>
+  </si>
+  <si>
+    <t>Pungangan, MAJENANG, KABUPATEN CILACAP, JAWA TENGAH</t>
+  </si>
+  <si>
+    <t>LIA ETIKASARI</t>
+  </si>
+  <si>
     <t>Tidak Ingin Menyebutkan</t>
   </si>
   <si>
-    <t>idafania33@gmail.com</t>
-  </si>
-  <si>
-    <t>OFF</t>
-  </si>
-  <si>
-    <t>LIA ETIKASARI</t>
-  </si>
-  <si>
     <t>liaetikasari0826@gmail.com</t>
   </si>
   <si>
     <t>KURNIA AINUN</t>
   </si>
   <si>
+    <t>Transgender</t>
+  </si>
+  <si>
     <t>etikasarilia26@gmail.com</t>
+  </si>
+  <si>
+    <t>Temanggung, 2003-03-03</t>
+  </si>
+  <si>
+    <t>KENANGAN, KOTAGEDE, KOTA YOGYAKARTA, DI YOGYAKARTA</t>
   </si>
 </sst>
 </file>
@@ -428,8 +440,8 @@
     <col min="2" max="2" width="28" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="31" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="83" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="31" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="90" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="10" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.10" bestFit="true" style="0"/>
     <col min="9" max="9" width="8" bestFit="true" customWidth="true" style="0"/>
@@ -492,19 +504,25 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
       <c r="D3">
         <v>6289907711225</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>56351</v>
+      </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -512,10 +530,10 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>85158040206</v>
@@ -529,20 +547,26 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>628885122711</v>
       </c>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>12345</v>
+      </c>
       <c r="I5" t="s">
         <v>13</v>
       </c>

</xml_diff>